<commit_message>
feat: draw type11 with svg phase 1
</commit_message>
<xml_diff>
--- a/assets/materials/11-安全彎鉤直/text.xlsx
+++ b/assets/materials/11-安全彎鉤直/text.xlsx
@@ -209,6 +209,36 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -615,7 +645,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="60" customHeight="1">
+    <row r="4" ht="120" customHeight="1">
       <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
@@ -633,12 +663,7 @@
       <c r="G4" s="4" t="n"/>
       <c r="H4" s="4" t="n"/>
       <c r="I4" s="4" t="n"/>
-      <c r="J4" s="5" t="inlineStr">
-        <is>
-          <t>直鋼筋 安#3-390x40
-長度: 390cm</t>
-        </is>
-      </c>
+      <c r="J4" s="5" t="inlineStr"/>
       <c r="K4" s="4" t="n">
         <v>390</v>
       </c>
@@ -711,7 +736,7 @@
     <row r="9">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-08-14 16:56:55 | 圖示功能：暫時停用，等 assets/materials 圖片準備好時再實作</t>
+          <t>生成時間：2025-08-14 17:30:28 | 圖示功能：暫時停用，等 assets/materials 圖片準備好時再實作</t>
         </is>
       </c>
     </row>
@@ -733,5 +758,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: use seperate sub processors
</commit_message>
<xml_diff>
--- a/assets/materials/11-安全彎鉤直/text.xlsx
+++ b/assets/materials/11-安全彎鉤直/text.xlsx
@@ -209,36 +209,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>3</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1905000" cy="1143000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -645,7 +615,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="120" customHeight="1">
+    <row r="4" ht="60" customHeight="1">
       <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
@@ -663,7 +633,12 @@
       <c r="G4" s="4" t="n"/>
       <c r="H4" s="4" t="n"/>
       <c r="I4" s="4" t="n"/>
-      <c r="J4" s="5" t="inlineStr"/>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>直鋼筋 安#3-390x40
+長度: 390cm</t>
+        </is>
+      </c>
       <c r="K4" s="4" t="n">
         <v>390</v>
       </c>
@@ -736,7 +711,7 @@
     <row r="9">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-08-14 17:30:28 | 圖示功能：暫時停用，等 assets/materials 圖片準備好時再實作</t>
+          <t>生成時間：2025-10-06 08:08:06 | 圖示功能：暫時停用，等 assets/materials 圖片準備好時再實作</t>
         </is>
       </c>
     </row>
@@ -758,6 +733,5 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add type 19
</commit_message>
<xml_diff>
--- a/assets/materials/11-安全彎鉤直/text.xlsx
+++ b/assets/materials/11-安全彎鉤直/text.xlsx
@@ -209,6 +209,36 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -615,7 +645,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="60" customHeight="1">
+    <row r="4" ht="120" customHeight="1">
       <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
@@ -633,12 +663,7 @@
       <c r="G4" s="4" t="n"/>
       <c r="H4" s="4" t="n"/>
       <c r="I4" s="4" t="n"/>
-      <c r="J4" s="5" t="inlineStr">
-        <is>
-          <t>直鋼筋 安#3-390x40
-長度: 390cm</t>
-        </is>
-      </c>
+      <c r="J4" s="5" t="inlineStr"/>
       <c r="K4" s="4" t="n">
         <v>390</v>
       </c>
@@ -711,7 +736,7 @@
     <row r="9">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-10-06 08:08:06 | 圖示功能：暫時停用，等 assets/materials 圖片準備好時再實作</t>
+          <t>生成時間：2025-10-06 08:36:04 | 圖示功能：已啟用 (mixed 模式)</t>
         </is>
       </c>
     </row>
@@ -733,5 +758,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>